<commit_message>
flare list, tasks, implementing event list function
</commit_message>
<xml_diff>
--- a/Data/x_flare_list.xlsx
+++ b/Data/x_flare_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="58">
   <si>
     <t>X1.5</t>
   </si>
@@ -199,6 +199,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyymmdd"/>
+    <numFmt numFmtId="165" formatCode="hh"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -251,23 +255,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -598,15 +606,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:H44"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:12">
       <c r="A1" s="5" t="s">
         <v>50</v>
       </c>
@@ -632,7 +640,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>40611</v>
       </c>
@@ -657,8 +665,19 @@
       <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J2" s="6">
+        <f>A2</f>
+        <v>40611</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <f>B2</f>
+        <v>0.96736111111111101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>40764</v>
       </c>
@@ -683,8 +702,19 @@
       <c r="H3" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="J3" s="6">
+        <f t="shared" ref="J3:J47" si="0">A3</f>
+        <v>40764</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" ref="L3:L47" si="1">B3</f>
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>40792</v>
       </c>
@@ -709,8 +739,19 @@
       <c r="H4" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="J4" s="6">
+        <f t="shared" si="0"/>
+        <v>40792</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="1"/>
+        <v>0.92499999999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>40808</v>
       </c>
@@ -733,8 +774,19 @@
       <c r="H5" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="J5" s="6">
+        <f t="shared" si="0"/>
+        <v>40808</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" si="1"/>
+        <v>0.4368055555555555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>40810</v>
       </c>
@@ -759,8 +811,19 @@
       <c r="H6" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="J6" s="6">
+        <f t="shared" si="0"/>
+        <v>40810</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="1"/>
+        <v>0.38958333333333334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>40850</v>
       </c>
@@ -785,8 +848,23 @@
       <c r="H7" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="J7" s="6">
+        <f t="shared" si="0"/>
+        <v>40850</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="7">
+        <f t="shared" si="1"/>
+        <v>0.84444444444444444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="J8" s="6"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>40935</v>
       </c>
@@ -811,8 +889,19 @@
       <c r="H9" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="J9" s="6">
+        <f t="shared" si="0"/>
+        <v>40935</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.73402777777777783</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>40975</v>
       </c>
@@ -835,8 +924,19 @@
       <c r="H10" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="J10" s="6">
+        <f t="shared" si="0"/>
+        <v>40975</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" si="1"/>
+        <v>1.3888888888888889E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>40975</v>
       </c>
@@ -861,8 +961,19 @@
       <c r="H11" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="J11" s="6">
+        <f t="shared" si="0"/>
+        <v>40975</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="1"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>41096</v>
       </c>
@@ -885,8 +996,19 @@
       <c r="H12" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="J12" s="6">
+        <f t="shared" si="0"/>
+        <v>41096</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" si="1"/>
+        <v>0.9590277777777777</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>41102</v>
       </c>
@@ -911,8 +1033,19 @@
       <c r="H13" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="J13" s="6">
+        <f t="shared" si="0"/>
+        <v>41102</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="1"/>
+        <v>0.65069444444444446</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>41205</v>
       </c>
@@ -935,8 +1068,23 @@
       <c r="H14" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="J14" s="6">
+        <f t="shared" si="0"/>
+        <v>41205</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.13402777777777777</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="J15" s="6"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>41407</v>
       </c>
@@ -959,8 +1107,19 @@
       <c r="H16" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="J16" s="6">
+        <f t="shared" si="0"/>
+        <v>41407</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="7">
+        <f t="shared" si="1"/>
+        <v>7.8472222222222221E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>41407</v>
       </c>
@@ -985,8 +1144,19 @@
       <c r="H17" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="J17" s="6">
+        <f t="shared" si="0"/>
+        <v>41407</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="7">
+        <f t="shared" si="1"/>
+        <v>0.65833333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>41408</v>
       </c>
@@ -1009,8 +1179,19 @@
       <c r="H18" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="J18" s="6">
+        <f t="shared" si="0"/>
+        <v>41408</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>41409</v>
       </c>
@@ -1035,8 +1216,19 @@
       <c r="H19" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="J19" s="6">
+        <f t="shared" si="0"/>
+        <v>41409</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="7">
+        <f t="shared" si="1"/>
+        <v>5.9027777777777783E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>41572</v>
       </c>
@@ -1059,8 +1251,19 @@
       <c r="H20" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="J20" s="6">
+        <f t="shared" si="0"/>
+        <v>41572</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" s="7">
+        <f t="shared" si="1"/>
+        <v>0.32847222222222222</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>41572</v>
       </c>
@@ -1083,8 +1286,19 @@
       <c r="H21" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="J21" s="6">
+        <f t="shared" si="0"/>
+        <v>41572</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L21" s="7">
+        <f t="shared" si="1"/>
+        <v>0.61875000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>41575</v>
       </c>
@@ -1109,8 +1323,19 @@
       <c r="H22" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="J22" s="6">
+        <f t="shared" si="0"/>
+        <v>41575</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" s="7">
+        <f t="shared" si="1"/>
+        <v>7.013888888888889E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>41576</v>
       </c>
@@ -1133,8 +1358,19 @@
       <c r="H23" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="J23" s="6">
+        <f t="shared" si="0"/>
+        <v>41576</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="7">
+        <f t="shared" si="1"/>
+        <v>0.90416666666666667</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>41583</v>
       </c>
@@ -1159,8 +1395,19 @@
       <c r="H24" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="J24" s="6">
+        <f t="shared" si="0"/>
+        <v>41583</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L24" s="7">
+        <f t="shared" si="1"/>
+        <v>0.92152777777777783</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>41586</v>
       </c>
@@ -1185,8 +1432,19 @@
       <c r="H25" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="J25" s="6">
+        <f t="shared" si="0"/>
+        <v>41586</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="7">
+        <f t="shared" si="1"/>
+        <v>0.18055555555555555</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>41588</v>
       </c>
@@ -1211,8 +1469,19 @@
       <c r="H26" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="J26" s="6">
+        <f t="shared" si="0"/>
+        <v>41588</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="7">
+        <f t="shared" si="1"/>
+        <v>0.21388888888888891</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>41597</v>
       </c>
@@ -1235,8 +1504,23 @@
       <c r="H27" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="J27" s="6">
+        <f t="shared" si="0"/>
+        <v>41597</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" s="7">
+        <f t="shared" si="1"/>
+        <v>0.42638888888888887</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="J28" s="6"/>
+      <c r="L28" s="7"/>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>41646</v>
       </c>
@@ -1259,8 +1543,19 @@
       <c r="H29" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="J29" s="6">
+        <f t="shared" si="0"/>
+        <v>41646</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" s="7">
+        <f t="shared" si="1"/>
+        <v>0.75277777777777777</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>41695</v>
       </c>
@@ -1285,8 +1580,19 @@
       <c r="H30" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="J30" s="6">
+        <f t="shared" si="0"/>
+        <v>41695</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L30" s="7">
+        <f t="shared" si="1"/>
+        <v>2.7083333333333334E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>41727</v>
       </c>
@@ -1311,8 +1617,19 @@
       <c r="H31" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="J31" s="6">
+        <f t="shared" si="0"/>
+        <v>41727</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" s="7">
+        <f t="shared" si="1"/>
+        <v>0.73263888888888884</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="1">
         <v>41754</v>
       </c>
@@ -1335,8 +1652,19 @@
       <c r="H32" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="J32" s="6">
+        <f t="shared" si="0"/>
+        <v>41754</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="7">
+        <f t="shared" si="1"/>
+        <v>1.1805555555555555E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="1">
         <v>41800</v>
       </c>
@@ -1361,8 +1689,19 @@
       <c r="H33" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="J33" s="6">
+        <f t="shared" si="0"/>
+        <v>41800</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L33" s="7">
+        <f t="shared" si="1"/>
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="1">
         <v>41800</v>
       </c>
@@ -1387,8 +1726,19 @@
       <c r="H34" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="J34" s="6">
+        <f t="shared" si="0"/>
+        <v>41800</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L34" s="7">
+        <f t="shared" si="1"/>
+        <v>0.48333333333333334</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="1">
         <v>41801</v>
       </c>
@@ -1413,8 +1763,19 @@
       <c r="H35" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="J35" s="6">
+        <f t="shared" si="0"/>
+        <v>41801</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" s="7">
+        <f t="shared" si="1"/>
+        <v>0.3743055555555555</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="1">
         <v>41892</v>
       </c>
@@ -1439,8 +1800,19 @@
       <c r="H36" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="J36" s="6">
+        <f t="shared" si="0"/>
+        <v>41892</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L36" s="7">
+        <f t="shared" si="1"/>
+        <v>0.72291666666666676</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="1">
         <v>41931</v>
       </c>
@@ -1463,8 +1835,19 @@
       <c r="H37" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="J37" s="6">
+        <f t="shared" si="0"/>
+        <v>41931</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L37" s="7">
+        <f t="shared" si="1"/>
+        <v>0.17847222222222223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" s="1">
         <v>41934</v>
       </c>
@@ -1489,8 +1872,19 @@
       <c r="H38" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="J38" s="6">
+        <f t="shared" si="0"/>
+        <v>41934</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L38" s="7">
+        <f t="shared" si="1"/>
+        <v>0.58472222222222225</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="1">
         <v>41936</v>
       </c>
@@ -1515,8 +1909,19 @@
       <c r="H39" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="J39" s="6">
+        <f t="shared" si="0"/>
+        <v>41936</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L39" s="7">
+        <f t="shared" si="1"/>
+        <v>0.87986111111111109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" s="1">
         <v>41937</v>
       </c>
@@ -1541,8 +1946,19 @@
       <c r="H40" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="J40" s="6">
+        <f t="shared" si="0"/>
+        <v>41937</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L40" s="7">
+        <f t="shared" si="1"/>
+        <v>0.70486111111111116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" s="1">
         <v>41938</v>
       </c>
@@ -1567,8 +1983,19 @@
       <c r="H41" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="J41" s="6">
+        <f t="shared" si="0"/>
+        <v>41938</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L41" s="7">
+        <f t="shared" si="1"/>
+        <v>0.41944444444444445</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="1">
         <v>41939</v>
       </c>
@@ -1593,8 +2020,19 @@
       <c r="H42" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="J42" s="6">
+        <f t="shared" si="0"/>
+        <v>41939</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L42" s="7">
+        <f t="shared" si="1"/>
+        <v>0.59166666666666667</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="1">
         <v>41950</v>
       </c>
@@ -1617,8 +2055,19 @@
       <c r="H43" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="J43" s="6">
+        <f t="shared" si="0"/>
+        <v>41950</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L43" s="7">
+        <f t="shared" si="1"/>
+        <v>0.70347222222222217</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="1">
         <v>41993</v>
       </c>
@@ -1643,8 +2092,23 @@
       <c r="H44" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="J44" s="6">
+        <f t="shared" si="0"/>
+        <v>41993</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L44" s="7">
+        <f t="shared" si="1"/>
+        <v>7.6388888888888886E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="J45" s="6"/>
+      <c r="L45" s="7"/>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" s="1">
         <v>42074</v>
       </c>
@@ -1669,8 +2133,19 @@
       <c r="H46" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="J46" s="6">
+        <f t="shared" si="0"/>
+        <v>42074</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L46" s="7">
+        <f t="shared" si="1"/>
+        <v>0.6743055555555556</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="1">
         <v>42129</v>
       </c>
@@ -1692,6 +2167,17 @@
       </c>
       <c r="H47" s="4" t="s">
         <v>2</v>
+      </c>
+      <c r="J47" s="6">
+        <f t="shared" si="0"/>
+        <v>42129</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L47" s="7">
+        <f t="shared" si="1"/>
+        <v>0.92013888888888884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new script to read event lists, reworked omni
</commit_message>
<xml_diff>
--- a/Data/x_flare_list.xlsx
+++ b/Data/x_flare_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
+    <workbookView xWindow="6380" yWindow="0" windowWidth="19220" windowHeight="14860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -255,9 +255,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -272,10 +273,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -609,7 +611,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>